<commit_message>
save summary stats into excel worksheet
</commit_message>
<xml_diff>
--- a/tables/tables.xlsx
+++ b/tables/tables.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="prop_id_by_ttwa" sheetId="1" r:id="rId1"/>
+    <sheet name="rci_by_year_place" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="35">
   <si>
     <t>2006-2007</t>
   </si>
@@ -101,14 +102,33 @@
   </si>
   <si>
     <t>TTWA</t>
+  </si>
+  <si>
+    <t>place</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>rci</t>
+  </si>
+  <si>
+    <t>rdi</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>pop_area_conc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -139,9 +159,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,7 +469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -902,4 +923,2085 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F103"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>2004</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.172225219900698</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.221781758685026</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.34092402315310699</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.30240670000294401</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>2004</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.18640663617764799</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.13541343947943699</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.39974550264297698</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.33486699442089901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>2004</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5.8297468249975896E-3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.13827045648335301</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.38713596938660699</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.31853558014084599</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2004</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.22968503348618499</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.14257769582915</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.39012685349381099</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.33398725124565898</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>2004</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.112895894504392</v>
+      </c>
+      <c r="D6" s="2">
+        <v>9.9130074791645401E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.38564845529562197</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.35328353541827301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2004</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.127264212439792</v>
+      </c>
+      <c r="D7" s="2">
+        <v>9.3299341340808001E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.35661335275976103</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.389669258573069</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>2004</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.30990609524229701</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.248111488420305</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.397798308246541</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.34120997024414002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>2004</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.166882794026876</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.14965263497676701</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.366334365397182</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.38926493692345199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2004</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.192245825817142</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.15865396821466601</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.34947752681171501</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.35977310993772899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>2004</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.33548550108108099</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.200980455124597</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.40835685239873398</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.32947110378338901</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>2004</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.30966449736507301</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.28555674249944601</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.39689600690923399</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.38913730502382499</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2004</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.18926228544981399</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.21200936822727201</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.38361543181341801</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.36661022327736398</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>2004</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.21382126133775101</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.12506961124872501</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.37824739824703102</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.38915796607784398</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>2004</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.206996646947195</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.25136669087493402</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.36329912398500003</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.37029775905207701</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>2004</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4.6105627548608398E-2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.17848018160338899</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.34447283837329401</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.34254386536023101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>2004</v>
+      </c>
+      <c r="C17" s="2">
+        <v>6.5284669135178594E-2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.147661016878153</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.32471313359014697</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.37405769606619199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>2004</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.18365310736451099</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.188371237399764</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.36136848232489599</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.36881379065172498</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>2004</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.8229478640284801E-2</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.178547029793683</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.33116668693455997</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.35489219172098502</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>2004</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.124731344842461</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.16063822251297599</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.32817310298063801</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.38151239880620802</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>2004</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.25747563504848597</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.23679587564418</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.36095965775998601</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.40639643568390799</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>2004</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.14007951026769799</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.202967119388827</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.32762783346163799</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.36606327698737701</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>2004</v>
+      </c>
+      <c r="C23" s="2">
+        <v>-8.2017109391684301E-2</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.15871778010139201</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.31323737279002201</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.35307790033088998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>2004</v>
+      </c>
+      <c r="C24" s="2">
+        <v>9.7745517086719094E-2</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.16396100336637601</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.29715745528072901</v>
+      </c>
+      <c r="F24" s="2">
+        <v>0.35223888984428098</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>2007</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.137974117767868</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.20412659311695899</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.33867982523379098</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.30312541266198101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>2007</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.156347925705141</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.16550133013079699</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.40411957966691098</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.335095648329018</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27">
+        <v>2007</v>
+      </c>
+      <c r="C27" s="2">
+        <v>-8.3898553474237598E-3</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.13292286859915201</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.38881149879985899</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.31653435010605202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>2007</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.21174776665028799</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.13308604827960299</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.37735642181760698</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.33222701235570301</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <v>2007</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.105485551371368</v>
+      </c>
+      <c r="D29" s="2">
+        <v>9.80655848782791E-2</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.38983402840417603</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.35176888163361603</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>2007</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.105273745949897</v>
+      </c>
+      <c r="D30" s="2">
+        <v>9.3671138353175906E-2</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.34910706226821497</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.38910200082241397</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>2007</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.33878932488492097</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.27521598636833999</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.40475475354108598</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.34018646399560698</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32">
+        <v>2007</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.16430552707569901</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.165154343646079</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.354266425788621</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.38800331891535</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>2007</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.17353710600637201</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.16728477569577599</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0.34952916834361503</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.35879053541136002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34">
+        <v>2007</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.309862345310087</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.19978290459826001</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0.39865002983931502</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.33062119425937497</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35">
+        <v>2007</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.33711528529297402</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.32183065017854801</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0.409787667007602</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.38809863844966902</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36">
+        <v>2007</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.162803700505569</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.205467216416059</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0.36114084658782603</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.366811511167979</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37">
+        <v>2007</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.173180016403614</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.11091743224705999</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.37183205662358598</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.389957961434657</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38">
+        <v>2007</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.229585679976063</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.26301252428891903</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0.36577861165898901</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.368511709792121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39">
+        <v>2007</v>
+      </c>
+      <c r="C39" s="2">
+        <v>4.3685562767446999E-2</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.16038396841817601</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0.329271753360941</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.34058572785409602</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40">
+        <v>2007</v>
+      </c>
+      <c r="C40" s="2">
+        <v>6.0366136786712002E-2</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.147212197759403</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0.31528048041571999</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.37268476812204798</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41">
+        <v>2007</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.16997031176966201</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.178224717522415</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0.34168233435990802</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.36611955783220401</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42">
+        <v>2007</v>
+      </c>
+      <c r="C42" s="2">
+        <v>7.3038854311241498E-3</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.18829049052702301</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0.32068994077914098</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.35357038119953499</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43">
+        <v>2007</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.111429078339813</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.151985733981335</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0.31797704909118701</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.38183432000380002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44">
+        <v>2007</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.204344347858645</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.21375665293000101</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0.33686316906078501</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.40662844045373198</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45">
+        <v>2007</v>
+      </c>
+      <c r="C45" s="2">
+        <v>9.7216037193722807E-2</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.18055314064581701</v>
+      </c>
+      <c r="E45" s="2">
+        <v>0.303238384926036</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0.36647979185736401</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46">
+        <v>2007</v>
+      </c>
+      <c r="C46" s="2">
+        <v>-7.8764171207945793E-2</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.13333499885983499</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0.29791241909006</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0.35211592116586099</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47">
+        <v>2007</v>
+      </c>
+      <c r="C47" s="2">
+        <v>9.861834848204E-2</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.15755862493966399</v>
+      </c>
+      <c r="E47" s="2">
+        <v>0.281696892224574</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0.35161667018715798</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48">
+        <v>2010</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.109182052324719</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.18296987110353799</v>
+      </c>
+      <c r="E48" s="2">
+        <v>0.32359764288700199</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0.30465399254272801</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49">
+        <v>2010</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.130855607447601</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.148346349731419</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0.379372542545997</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.33547386346235702</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50">
+        <v>2010</v>
+      </c>
+      <c r="C50" s="2">
+        <v>-8.8742917511463997E-3</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.132207506019518</v>
+      </c>
+      <c r="E50" s="2">
+        <v>0.37781058803650902</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0.31575006453985999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51">
+        <v>2010</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.19509735222308899</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.123165082697151</v>
+      </c>
+      <c r="E51" s="2">
+        <v>0.365677109196891</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0.331330948095936</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52">
+        <v>2010</v>
+      </c>
+      <c r="C52" s="2">
+        <v>7.9482701191906396E-2</v>
+      </c>
+      <c r="D52" s="2">
+        <v>9.4193781559717402E-2</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0.377093295635748</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0.35204122539876098</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53">
+        <v>2010</v>
+      </c>
+      <c r="C53" s="2">
+        <v>9.1599040251907293E-2</v>
+      </c>
+      <c r="D53" s="2">
+        <v>8.9593576722150695E-2</v>
+      </c>
+      <c r="E53" s="2">
+        <v>0.337799150975093</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0.38906534517267199</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>2010</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.28986080576856998</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0.25027055461359399</v>
+      </c>
+      <c r="E54" s="2">
+        <v>0.37589671437448402</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0.33981223218470702</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55">
+        <v>2010</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.15095255986341199</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.157183437074532</v>
+      </c>
+      <c r="E55" s="2">
+        <v>0.33782303270029401</v>
+      </c>
+      <c r="F55" s="2">
+        <v>0.38746176545712102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56">
+        <v>2010</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.171560408291141</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.16667657097008901</v>
+      </c>
+      <c r="E56" s="2">
+        <v>0.33619318021302103</v>
+      </c>
+      <c r="F56" s="2">
+        <v>0.35836144682663401</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57">
+        <v>2010</v>
+      </c>
+      <c r="C57" s="2">
+        <v>0.27139767143447702</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.17412157947175699</v>
+      </c>
+      <c r="E57" s="2">
+        <v>0.38481030123194099</v>
+      </c>
+      <c r="F57" s="2">
+        <v>0.33167078191343702</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58">
+        <v>2010</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0.30326906617514399</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.29534708707775298</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0.38162522836976698</v>
+      </c>
+      <c r="F58" s="2">
+        <v>0.38897885105922703</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59">
+        <v>2010</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0.12586341887758901</v>
+      </c>
+      <c r="D59" s="2">
+        <v>0.18720044916071699</v>
+      </c>
+      <c r="E59" s="2">
+        <v>0.34389413856204898</v>
+      </c>
+      <c r="F59" s="2">
+        <v>0.36712890202278398</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>18</v>
+      </c>
+      <c r="B60">
+        <v>2010</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.160234419607518</v>
+      </c>
+      <c r="D60" s="2">
+        <v>0.108673253081527</v>
+      </c>
+      <c r="E60" s="2">
+        <v>0.36616422726701298</v>
+      </c>
+      <c r="F60" s="2">
+        <v>0.39103343086765402</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61">
+        <v>2010</v>
+      </c>
+      <c r="C61" s="2">
+        <v>0.222374950620079</v>
+      </c>
+      <c r="D61" s="2">
+        <v>0.23717586729821899</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0.34393956942661402</v>
+      </c>
+      <c r="F61" s="2">
+        <v>0.36911990328484701</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62">
+        <v>2010</v>
+      </c>
+      <c r="C62" s="2">
+        <v>4.75322876798129E-2</v>
+      </c>
+      <c r="D62" s="2">
+        <v>0.15758081599943499</v>
+      </c>
+      <c r="E62" s="2">
+        <v>0.32758422903238599</v>
+      </c>
+      <c r="F62" s="2">
+        <v>0.34005528555099102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63">
+        <v>2010</v>
+      </c>
+      <c r="C63" s="2">
+        <v>5.2380111646006103E-2</v>
+      </c>
+      <c r="D63" s="2">
+        <v>0.14188059083715099</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0.30915718799645497</v>
+      </c>
+      <c r="F63" s="2">
+        <v>0.37203648677806</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>25</v>
+      </c>
+      <c r="B64">
+        <v>2010</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0.175100882716129</v>
+      </c>
+      <c r="D64" s="2">
+        <v>0.18128841048731201</v>
+      </c>
+      <c r="E64" s="2">
+        <v>0.34029154708911202</v>
+      </c>
+      <c r="F64" s="2">
+        <v>0.36637722551123902</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>27</v>
+      </c>
+      <c r="B65">
+        <v>2010</v>
+      </c>
+      <c r="C65" s="2">
+        <v>1.36393028190849E-2</v>
+      </c>
+      <c r="D65" s="2">
+        <v>0.18380721808570399</v>
+      </c>
+      <c r="E65" s="2">
+        <v>0.31999032456654303</v>
+      </c>
+      <c r="F65" s="2">
+        <v>0.35370395542819399</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66">
+        <v>2010</v>
+      </c>
+      <c r="C66" s="2">
+        <v>0.122821779704913</v>
+      </c>
+      <c r="D66" s="2">
+        <v>0.15478943304812401</v>
+      </c>
+      <c r="E66" s="2">
+        <v>0.31412953212927602</v>
+      </c>
+      <c r="F66" s="2">
+        <v>0.382555774702382</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67">
+        <v>2010</v>
+      </c>
+      <c r="C67" s="2">
+        <v>0.205609938834348</v>
+      </c>
+      <c r="D67" s="2">
+        <v>0.20625920785646101</v>
+      </c>
+      <c r="E67" s="2">
+        <v>0.33481445696133</v>
+      </c>
+      <c r="F67" s="2">
+        <v>0.407392520540312</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>24</v>
+      </c>
+      <c r="B68">
+        <v>2010</v>
+      </c>
+      <c r="C68" s="2">
+        <v>0.10089370619337</v>
+      </c>
+      <c r="D68" s="2">
+        <v>0.174266884456514</v>
+      </c>
+      <c r="E68" s="2">
+        <v>0.29443394259768102</v>
+      </c>
+      <c r="F68" s="2">
+        <v>0.36744859331457702</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69">
+        <v>2010</v>
+      </c>
+      <c r="C69" s="2">
+        <v>-9.8736144758254402E-2</v>
+      </c>
+      <c r="D69" s="2">
+        <v>0.13171475893681001</v>
+      </c>
+      <c r="E69" s="2">
+        <v>0.29456861337442602</v>
+      </c>
+      <c r="F69" s="2">
+        <v>0.351793695299848</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>26</v>
+      </c>
+      <c r="B70">
+        <v>2010</v>
+      </c>
+      <c r="C70" s="2">
+        <v>0.10355227811357599</v>
+      </c>
+      <c r="D70" s="2">
+        <v>0.161411497654282</v>
+      </c>
+      <c r="E70" s="2">
+        <v>0.28225273785791599</v>
+      </c>
+      <c r="F70" s="2">
+        <v>0.35311764083716601</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71">
+        <v>2015</v>
+      </c>
+      <c r="C71" s="2">
+        <v>9.7177174902090394E-2</v>
+      </c>
+      <c r="D71" s="2">
+        <v>0.17076735898946399</v>
+      </c>
+      <c r="E71" s="2">
+        <v>0.33624679663356799</v>
+      </c>
+      <c r="F71" s="2">
+        <v>0.36728253853335802</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>24</v>
+      </c>
+      <c r="B72">
+        <v>2015</v>
+      </c>
+      <c r="C72" s="2">
+        <v>8.0218555783745898E-2</v>
+      </c>
+      <c r="D72" s="2">
+        <v>0.16473743898736501</v>
+      </c>
+      <c r="E72" s="2">
+        <v>0.29436266487888102</v>
+      </c>
+      <c r="F72" s="2">
+        <v>0.37054034645645201</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>21</v>
+      </c>
+      <c r="B73">
+        <v>2015</v>
+      </c>
+      <c r="C73" s="2">
+        <v>0.187805877470021</v>
+      </c>
+      <c r="D73" s="2">
+        <v>0.20355998375849699</v>
+      </c>
+      <c r="E73" s="2">
+        <v>0.31003304344645999</v>
+      </c>
+      <c r="F73" s="2">
+        <v>0.37249224192827302</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74">
+        <v>2015</v>
+      </c>
+      <c r="C74" s="2">
+        <v>8.2904649861500798E-2</v>
+      </c>
+      <c r="D74" s="2">
+        <v>0.15420861652815901</v>
+      </c>
+      <c r="E74" s="2">
+        <v>0.27728535183727998</v>
+      </c>
+      <c r="F74" s="2">
+        <v>0.30442775483281698</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>15</v>
+      </c>
+      <c r="B75">
+        <v>2015</v>
+      </c>
+      <c r="C75" s="2">
+        <v>2.94651310556301E-2</v>
+      </c>
+      <c r="D75" s="2">
+        <v>0.16394125957337799</v>
+      </c>
+      <c r="E75" s="2">
+        <v>0.31872078325054898</v>
+      </c>
+      <c r="F75" s="2">
+        <v>0.34152378236424602</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>18</v>
+      </c>
+      <c r="B76">
+        <v>2015</v>
+      </c>
+      <c r="C76" s="2">
+        <v>0.15635290631245199</v>
+      </c>
+      <c r="D76" s="2">
+        <v>0.12967686698203201</v>
+      </c>
+      <c r="E76" s="2">
+        <v>0.35382176454234698</v>
+      </c>
+      <c r="F76" s="2">
+        <v>0.39064960898307799</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77">
+        <v>2015</v>
+      </c>
+      <c r="C77" s="2">
+        <v>0.22318507601998999</v>
+      </c>
+      <c r="D77" s="2">
+        <v>0.22097946069951899</v>
+      </c>
+      <c r="E77" s="2">
+        <v>0.345930526140378</v>
+      </c>
+      <c r="F77" s="2">
+        <v>0.34177276459658401</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>16</v>
+      </c>
+      <c r="B78">
+        <v>2015</v>
+      </c>
+      <c r="C78" s="2">
+        <v>0.24209692171677699</v>
+      </c>
+      <c r="D78" s="2">
+        <v>0.252722506707038</v>
+      </c>
+      <c r="E78" s="2">
+        <v>0.33760570330934903</v>
+      </c>
+      <c r="F78" s="2">
+        <v>0.38984466345959201</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>7</v>
+      </c>
+      <c r="B79">
+        <v>2015</v>
+      </c>
+      <c r="C79" s="2">
+        <v>0.107776469209358</v>
+      </c>
+      <c r="D79" s="2">
+        <v>0.13205745334087499</v>
+      </c>
+      <c r="E79" s="2">
+        <v>0.351745545941474</v>
+      </c>
+      <c r="F79" s="2">
+        <v>0.33690870566876002</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>25</v>
+      </c>
+      <c r="B80">
+        <v>2015</v>
+      </c>
+      <c r="C80" s="2">
+        <v>0.16941571011196299</v>
+      </c>
+      <c r="D80" s="2">
+        <v>0.19079566555416799</v>
+      </c>
+      <c r="E80" s="2">
+        <v>0.322226867660239</v>
+      </c>
+      <c r="F80" s="2">
+        <v>0.36579615635609197</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>27</v>
+      </c>
+      <c r="B81">
+        <v>2015</v>
+      </c>
+      <c r="C81" s="2">
+        <v>3.3038093106174701E-3</v>
+      </c>
+      <c r="D81" s="2">
+        <v>0.18979636102463901</v>
+      </c>
+      <c r="E81" s="2">
+        <v>0.30591529210665203</v>
+      </c>
+      <c r="F81" s="2">
+        <v>0.35564032218444103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>13</v>
+      </c>
+      <c r="B82">
+        <v>2015</v>
+      </c>
+      <c r="C82" s="2">
+        <v>0.25083570601741401</v>
+      </c>
+      <c r="D82" s="2">
+        <v>0.18447785962135699</v>
+      </c>
+      <c r="E82" s="2">
+        <v>0.38722576052332303</v>
+      </c>
+      <c r="F82" s="2">
+        <v>0.32851410113524299</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83">
+        <v>2015</v>
+      </c>
+      <c r="C83" s="2">
+        <v>-0.110499528736834</v>
+      </c>
+      <c r="D83" s="2">
+        <v>0.12026836672692399</v>
+      </c>
+      <c r="E83" s="2">
+        <v>0.28016067689430102</v>
+      </c>
+      <c r="F83" s="2">
+        <v>0.357994301450278</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>9</v>
+      </c>
+      <c r="B84">
+        <v>2015</v>
+      </c>
+      <c r="C84" s="2">
+        <v>0.16466834488884999</v>
+      </c>
+      <c r="D84" s="2">
+        <v>0.17575433160399501</v>
+      </c>
+      <c r="E84" s="2">
+        <v>0.31698129894427601</v>
+      </c>
+      <c r="F84" s="2">
+        <v>0.35813413707831498</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>11</v>
+      </c>
+      <c r="B85">
+        <v>2015</v>
+      </c>
+      <c r="C85" s="2">
+        <v>-3.8367447485633298E-3</v>
+      </c>
+      <c r="D85" s="2">
+        <v>0.14109069406015201</v>
+      </c>
+      <c r="E85" s="2">
+        <v>0.35810554519198801</v>
+      </c>
+      <c r="F85" s="2">
+        <v>0.31500836310682401</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>26</v>
+      </c>
+      <c r="B86">
+        <v>2015</v>
+      </c>
+      <c r="C86" s="2">
+        <v>0.12308530817164499</v>
+      </c>
+      <c r="D86" s="2">
+        <v>0.16238596664287799</v>
+      </c>
+      <c r="E86" s="2">
+        <v>0.26437648692992999</v>
+      </c>
+      <c r="F86" s="2">
+        <v>0.35347618554805499</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>20</v>
+      </c>
+      <c r="B87">
+        <v>2015</v>
+      </c>
+      <c r="C87" s="2">
+        <v>0.12633255325725901</v>
+      </c>
+      <c r="D87" s="2">
+        <v>0.16235332939573699</v>
+      </c>
+      <c r="E87" s="2">
+        <v>0.30746189411101499</v>
+      </c>
+      <c r="F87" s="2">
+        <v>0.38134140913328302</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88">
+        <v>2015</v>
+      </c>
+      <c r="C88" s="2">
+        <v>6.1741067589381797E-2</v>
+      </c>
+      <c r="D88" s="2">
+        <v>8.5011662112590702E-2</v>
+      </c>
+      <c r="E88" s="2">
+        <v>0.32455901168048401</v>
+      </c>
+      <c r="F88" s="2">
+        <v>0.388035656494361</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>14</v>
+      </c>
+      <c r="B89">
+        <v>2015</v>
+      </c>
+      <c r="C89" s="2">
+        <v>0.13284522276483099</v>
+      </c>
+      <c r="D89" s="2">
+        <v>0.15082085417458299</v>
+      </c>
+      <c r="E89" s="2">
+        <v>0.32042275391007102</v>
+      </c>
+      <c r="F89" s="2">
+        <v>0.38790563687285101</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>10</v>
+      </c>
+      <c r="B90">
+        <v>2015</v>
+      </c>
+      <c r="C90" s="2">
+        <v>4.63072722326121E-2</v>
+      </c>
+      <c r="D90" s="2">
+        <v>8.3740401545982501E-2</v>
+      </c>
+      <c r="E90" s="2">
+        <v>0.37188211766012302</v>
+      </c>
+      <c r="F90" s="2">
+        <v>0.353369329025635</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>22</v>
+      </c>
+      <c r="B91">
+        <v>2015</v>
+      </c>
+      <c r="C91" s="2">
+        <v>0.20749774230170501</v>
+      </c>
+      <c r="D91" s="2">
+        <v>0.208236632326292</v>
+      </c>
+      <c r="E91" s="2">
+        <v>0.32692216503939697</v>
+      </c>
+      <c r="F91" s="2">
+        <v>0.40789071886466</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>19</v>
+      </c>
+      <c r="B92">
+        <v>2015</v>
+      </c>
+      <c r="C92" s="2">
+        <v>4.9719157341570397E-2</v>
+      </c>
+      <c r="D92" s="2">
+        <v>0.157914920987378</v>
+      </c>
+      <c r="E92" s="2">
+        <v>0.296071624538707</v>
+      </c>
+      <c r="F92" s="2">
+        <v>0.37353318682439901</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>3</v>
+      </c>
+      <c r="B93">
+        <v>2015</v>
+      </c>
+      <c r="C93" s="2">
+        <v>0.153808336644604</v>
+      </c>
+      <c r="D93" s="2">
+        <v>0.12305282158400201</v>
+      </c>
+      <c r="E93" s="2">
+        <v>0.34765932733233301</v>
+      </c>
+      <c r="F93" s="2">
+        <v>0.333041736918047</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>4</v>
+      </c>
+      <c r="B94">
+        <v>2004</v>
+      </c>
+      <c r="C94" s="2">
+        <v>0.193422577577434</v>
+      </c>
+      <c r="D94" s="2">
+        <v>0.101776424375752</v>
+      </c>
+      <c r="E94" s="2">
+        <v>0.38328146095867299</v>
+      </c>
+      <c r="F94" s="2">
+        <v>0.40488406957999501</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>4</v>
+      </c>
+      <c r="B95">
+        <v>2006</v>
+      </c>
+      <c r="C95" s="2">
+        <v>0.18262574274179499</v>
+      </c>
+      <c r="D95" s="2">
+        <v>9.4081395144576294E-2</v>
+      </c>
+      <c r="E95" s="2">
+        <v>0.36279905286585701</v>
+      </c>
+      <c r="F95" s="2">
+        <v>0.40368595137207902</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>4</v>
+      </c>
+      <c r="B96">
+        <v>2009</v>
+      </c>
+      <c r="C96" s="2">
+        <v>0.16589685826818101</v>
+      </c>
+      <c r="D96" s="2">
+        <v>9.1220209990948001E-2</v>
+      </c>
+      <c r="E96" s="2">
+        <v>0.34682250070729298</v>
+      </c>
+      <c r="F96" s="2">
+        <v>0.40309294071818702</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>4</v>
+      </c>
+      <c r="B97">
+        <v>2012</v>
+      </c>
+      <c r="C97" s="2">
+        <v>0.12898476269776901</v>
+      </c>
+      <c r="D97" s="2">
+        <v>6.9110290331053106E-2</v>
+      </c>
+      <c r="E97" s="2">
+        <v>0.32850956945457099</v>
+      </c>
+      <c r="F97" s="2">
+        <v>0.401948586568668</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>17</v>
+      </c>
+      <c r="B98">
+        <v>2004</v>
+      </c>
+      <c r="C98" s="2">
+        <v>2.2302157206175899E-2</v>
+      </c>
+      <c r="D98" s="2">
+        <v>0.14783315213995399</v>
+      </c>
+      <c r="E98" s="2">
+        <v>0.38334638322457198</v>
+      </c>
+      <c r="F98" s="2">
+        <v>0.452366347306151</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>17</v>
+      </c>
+      <c r="B99">
+        <v>2006</v>
+      </c>
+      <c r="C99" s="2">
+        <v>1.7750642362878901E-2</v>
+      </c>
+      <c r="D99" s="2">
+        <v>0.13433434134776701</v>
+      </c>
+      <c r="E99" s="2">
+        <v>0.357843748405689</v>
+      </c>
+      <c r="F99" s="2">
+        <v>0.45186113705987302</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>17</v>
+      </c>
+      <c r="B100">
+        <v>2009</v>
+      </c>
+      <c r="C100" s="2">
+        <v>-8.1772726732204405E-3</v>
+      </c>
+      <c r="D100" s="2">
+        <v>0.114197560719851</v>
+      </c>
+      <c r="E100" s="2">
+        <v>0.33836551123829001</v>
+      </c>
+      <c r="F100" s="2">
+        <v>0.45170254554060402</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>17</v>
+      </c>
+      <c r="B101">
+        <v>2012</v>
+      </c>
+      <c r="C101" s="2">
+        <v>-2.91489385592726E-2</v>
+      </c>
+      <c r="D101" s="2">
+        <v>9.1862082443192994E-2</v>
+      </c>
+      <c r="E101" s="2">
+        <v>0.311234989269076</v>
+      </c>
+      <c r="F101" s="2">
+        <v>0.45176877169408902</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102">
+        <v>2016</v>
+      </c>
+      <c r="C102" s="2">
+        <v>0.12813359205511801</v>
+      </c>
+      <c r="D102" s="2">
+        <v>9.9174074364617004E-2</v>
+      </c>
+      <c r="E102" s="2">
+        <v>0.36708280092840401</v>
+      </c>
+      <c r="F102" s="2">
+        <v>0.40092096365954699</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>17</v>
+      </c>
+      <c r="B103">
+        <v>2016</v>
+      </c>
+      <c r="C103" s="2">
+        <v>-5.3406825562403601E-2</v>
+      </c>
+      <c r="D103" s="2">
+        <v>0.107341877740553</v>
+      </c>
+      <c r="E103" s="2">
+        <v>0.37423586226247502</v>
+      </c>
+      <c r="F103" s="2">
+        <v>0.44866021332749301</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add plots of change in id and non id by decile of distance and density
</commit_message>
<xml_diff>
--- a/tables/tables.xlsx
+++ b/tables/tables.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="prop_id_by_ttwa" sheetId="1" r:id="rId1"/>
     <sheet name="rci_by_year_place" sheetId="2" r:id="rId2"/>
+    <sheet name="ttwa_pop_sizes" sheetId="4" r:id="rId3"/>
+    <sheet name="cor_between_rci_rdi" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="37">
   <si>
     <t>2006-2007</t>
   </si>
@@ -121,16 +123,31 @@
   <si>
     <t>pop_area_conc</t>
   </si>
+  <si>
+    <t>pop_id</t>
+  </si>
+  <si>
+    <t>pop_total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,15 +173,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -929,7 +949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -3004,4 +3024,2173 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D103"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>2004</v>
+      </c>
+      <c r="C2" s="3">
+        <v>304533.36057940702</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1556306.54911039</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2007</v>
+      </c>
+      <c r="C3" s="3">
+        <v>356371.70182664599</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1581687.4878793899</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2010</v>
+      </c>
+      <c r="C4" s="3">
+        <v>335851.761428834</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1602194.9737682</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>2015</v>
+      </c>
+      <c r="C5" s="3">
+        <v>346325.52799999999</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1718366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>2004</v>
+      </c>
+      <c r="C6" s="3">
+        <v>86421.009953184301</v>
+      </c>
+      <c r="D6" s="3">
+        <v>737515.74452386901</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>2007</v>
+      </c>
+      <c r="C7" s="3">
+        <v>96245.814221157707</v>
+      </c>
+      <c r="D7" s="3">
+        <v>770839.18450519198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>2010</v>
+      </c>
+      <c r="C8" s="3">
+        <v>95343.235985840103</v>
+      </c>
+      <c r="D8" s="3">
+        <v>802126.38687950396</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>2015</v>
+      </c>
+      <c r="C9" s="3">
+        <v>103844.057</v>
+      </c>
+      <c r="D9" s="3">
+        <v>815882</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>2004</v>
+      </c>
+      <c r="C10" s="3">
+        <v>43672.481891881704</v>
+      </c>
+      <c r="D10" s="3">
+        <v>618790.55126791599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>2007</v>
+      </c>
+      <c r="C11" s="3">
+        <v>56070</v>
+      </c>
+      <c r="D11" s="3">
+        <v>638201.26901874295</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>2010</v>
+      </c>
+      <c r="C12" s="3">
+        <v>54957.590959206202</v>
+      </c>
+      <c r="D12" s="3">
+        <v>661110.44101433305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>2015</v>
+      </c>
+      <c r="C13" s="3">
+        <v>59063.163999999997</v>
+      </c>
+      <c r="D13" s="3">
+        <v>696114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>2004</v>
+      </c>
+      <c r="C14" s="3">
+        <v>78623.755242473897</v>
+      </c>
+      <c r="D14" s="3">
+        <v>553984.47274023003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>2007</v>
+      </c>
+      <c r="C15" s="3">
+        <v>89916.137474196701</v>
+      </c>
+      <c r="D15" s="3">
+        <v>560163.11236549704</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>2010</v>
+      </c>
+      <c r="C16" s="3">
+        <v>89353.741165075495</v>
+      </c>
+      <c r="D16" s="3">
+        <v>570509.201887473</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>2015</v>
+      </c>
+      <c r="C17" s="3">
+        <v>91768.426999999996</v>
+      </c>
+      <c r="D17" s="3">
+        <v>598635</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>2004</v>
+      </c>
+      <c r="C18" s="3">
+        <v>34077.346648773098</v>
+      </c>
+      <c r="D18" s="3">
+        <v>563650</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>2007</v>
+      </c>
+      <c r="C19" s="3">
+        <v>44460</v>
+      </c>
+      <c r="D19" s="3">
+        <v>570531</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>2010</v>
+      </c>
+      <c r="C20" s="3">
+        <v>43795</v>
+      </c>
+      <c r="D20" s="3">
+        <v>586577</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>2015</v>
+      </c>
+      <c r="C21" s="3">
+        <v>48009.468999999997</v>
+      </c>
+      <c r="D21" s="3">
+        <v>612642</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <v>2004</v>
+      </c>
+      <c r="C22" s="3">
+        <v>33162.232613335902</v>
+      </c>
+      <c r="D22" s="3">
+        <v>603287.363164793</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23">
+        <v>2007</v>
+      </c>
+      <c r="C23" s="3">
+        <v>43487.032729689301</v>
+      </c>
+      <c r="D23" s="3">
+        <v>605701.728009452</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>2010</v>
+      </c>
+      <c r="C24" s="3">
+        <v>41347.8452493031</v>
+      </c>
+      <c r="D24" s="3">
+        <v>618603.40103253303</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>2015</v>
+      </c>
+      <c r="C25" s="3">
+        <v>46525.025999999998</v>
+      </c>
+      <c r="D25" s="3">
+        <v>645884</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>2004</v>
+      </c>
+      <c r="C26" s="3">
+        <v>106429.381345881</v>
+      </c>
+      <c r="D26" s="3">
+        <v>743218.86691254796</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <v>2007</v>
+      </c>
+      <c r="C27" s="3">
+        <v>116775.049935619</v>
+      </c>
+      <c r="D27" s="3">
+        <v>768274.40438574401</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>2010</v>
+      </c>
+      <c r="C28" s="3">
+        <v>113159.088072238</v>
+      </c>
+      <c r="D28" s="3">
+        <v>805998.11491948203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29">
+        <v>2015</v>
+      </c>
+      <c r="C29" s="3">
+        <v>123732.39</v>
+      </c>
+      <c r="D29" s="3">
+        <v>793331</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <v>2004</v>
+      </c>
+      <c r="C30" s="3">
+        <v>104514.611684673</v>
+      </c>
+      <c r="D30" s="3">
+        <v>841437.29538845003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>2007</v>
+      </c>
+      <c r="C31" s="3">
+        <v>128156.967179061</v>
+      </c>
+      <c r="D31" s="3">
+        <v>862567.02077274595</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32">
+        <v>2010</v>
+      </c>
+      <c r="C32" s="3">
+        <v>123355.604486913</v>
+      </c>
+      <c r="D32" s="3">
+        <v>891690.83631076</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33">
+        <v>2015</v>
+      </c>
+      <c r="C33" s="3">
+        <v>127979.268</v>
+      </c>
+      <c r="D33" s="3">
+        <v>934173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>2004</v>
+      </c>
+      <c r="C34" s="3">
+        <v>240224.786299536</v>
+      </c>
+      <c r="D34" s="3">
+        <v>961172.06170341105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>2007</v>
+      </c>
+      <c r="C35" s="3">
+        <v>229949.986575727</v>
+      </c>
+      <c r="D35" s="3">
+        <v>953797.04653070704</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>2010</v>
+      </c>
+      <c r="C36" s="3">
+        <v>218619.69483640799</v>
+      </c>
+      <c r="D36" s="3">
+        <v>953031.08566804498</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>2015</v>
+      </c>
+      <c r="C37" s="3">
+        <v>222676.704</v>
+      </c>
+      <c r="D37" s="3">
+        <v>984327</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <v>2004</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1245816.2721307799</v>
+      </c>
+      <c r="D38" s="3">
+        <v>7178082.4968648404</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>2007</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1466880.90721883</v>
+      </c>
+      <c r="D39" s="3">
+        <v>7333943.7484442601</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40">
+        <v>2010</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1323152.19970478</v>
+      </c>
+      <c r="D40" s="3">
+        <v>7209890.8184753899</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41">
+        <v>2015</v>
+      </c>
+      <c r="C41" s="3">
+        <v>1349863.0220000001</v>
+      </c>
+      <c r="D41" s="3">
+        <v>8143569</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42">
+        <v>2004</v>
+      </c>
+      <c r="C42" s="3">
+        <v>65586.473353858702</v>
+      </c>
+      <c r="D42" s="3">
+        <v>656550</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43">
+        <v>2007</v>
+      </c>
+      <c r="C43" s="3">
+        <v>85910</v>
+      </c>
+      <c r="D43" s="3">
+        <v>661320</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44">
+        <v>2010</v>
+      </c>
+      <c r="C44" s="3">
+        <v>81500</v>
+      </c>
+      <c r="D44" s="3">
+        <v>676174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45">
+        <v>2015</v>
+      </c>
+      <c r="C45" s="3">
+        <v>84146.201000000001</v>
+      </c>
+      <c r="D45" s="3">
+        <v>717523</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46">
+        <v>2004</v>
+      </c>
+      <c r="C46" s="3">
+        <v>433784.35483774502</v>
+      </c>
+      <c r="D46" s="3">
+        <v>2441574.3013207698</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47">
+        <v>2007</v>
+      </c>
+      <c r="C47" s="3">
+        <v>487225.91888101801</v>
+      </c>
+      <c r="D47" s="3">
+        <v>2471593.6125626201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48">
+        <v>2010</v>
+      </c>
+      <c r="C48" s="3">
+        <v>460605.98137511301</v>
+      </c>
+      <c r="D48" s="3">
+        <v>2510095.6154284999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49">
+        <v>2015</v>
+      </c>
+      <c r="C49" s="3">
+        <v>478532.54800000001</v>
+      </c>
+      <c r="D49" s="3">
+        <v>2632304</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50">
+        <v>2004</v>
+      </c>
+      <c r="C50" s="3">
+        <v>61339.705086183603</v>
+      </c>
+      <c r="D50" s="3">
+        <v>546550.66453098506</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51">
+        <v>2007</v>
+      </c>
+      <c r="C51" s="3">
+        <v>73615.605216957105</v>
+      </c>
+      <c r="D51" s="3">
+        <v>558793.51346379798</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52">
+        <v>2010</v>
+      </c>
+      <c r="C52" s="3">
+        <v>72318.255610973501</v>
+      </c>
+      <c r="D52" s="3">
+        <v>571511.28001591004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53">
+        <v>2015</v>
+      </c>
+      <c r="C53" s="3">
+        <v>83469.807000000001</v>
+      </c>
+      <c r="D53" s="3">
+        <v>608030</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54">
+        <v>2004</v>
+      </c>
+      <c r="C54" s="3">
+        <v>191732.13427347201</v>
+      </c>
+      <c r="D54" s="3">
+        <v>994331.69124720001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55">
+        <v>2007</v>
+      </c>
+      <c r="C55" s="3">
+        <v>193206.99325648401</v>
+      </c>
+      <c r="D55" s="3">
+        <v>1004980.0375774699</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56">
+        <v>2010</v>
+      </c>
+      <c r="C56" s="3">
+        <v>184296.559108302</v>
+      </c>
+      <c r="D56" s="3">
+        <v>1017401.16721931</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57">
+        <v>2015</v>
+      </c>
+      <c r="C57" s="3">
+        <v>187783.9</v>
+      </c>
+      <c r="D57" s="3">
+        <v>1045244</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58">
+        <v>2004</v>
+      </c>
+      <c r="C58" s="3">
+        <v>112861.562729375</v>
+      </c>
+      <c r="D58" s="3">
+        <v>738787.81586655695</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59">
+        <v>2007</v>
+      </c>
+      <c r="C59" s="3">
+        <v>119208.213323761</v>
+      </c>
+      <c r="D59" s="3">
+        <v>758993.47190723999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60">
+        <v>2010</v>
+      </c>
+      <c r="C60" s="3">
+        <v>115843.83558713501</v>
+      </c>
+      <c r="D60" s="3">
+        <v>778295.20264208398</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61">
+        <v>2015</v>
+      </c>
+      <c r="C61" s="3">
+        <v>126877.67600000001</v>
+      </c>
+      <c r="D61" s="3">
+        <v>803369</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62">
+        <v>2004</v>
+      </c>
+      <c r="C62" s="3">
+        <v>33481.497655548803</v>
+      </c>
+      <c r="D62" s="3">
+        <v>497639.37715169601</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63">
+        <v>2007</v>
+      </c>
+      <c r="C63" s="3">
+        <v>42048.956744442497</v>
+      </c>
+      <c r="D63" s="3">
+        <v>518238.02450814401</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64">
+        <v>2010</v>
+      </c>
+      <c r="C64" s="3">
+        <v>40651.092713973798</v>
+      </c>
+      <c r="D64" s="3">
+        <v>522718.50040952797</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>24</v>
+      </c>
+      <c r="B65">
+        <v>2015</v>
+      </c>
+      <c r="C65" s="3">
+        <v>43294.2</v>
+      </c>
+      <c r="D65" s="3">
+        <v>548639</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66">
+        <v>2004</v>
+      </c>
+      <c r="C66" s="3">
+        <v>55748.938191397203</v>
+      </c>
+      <c r="D66" s="3">
+        <v>510205.80641997099</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67">
+        <v>2007</v>
+      </c>
+      <c r="C67" s="3">
+        <v>65231.751958054898</v>
+      </c>
+      <c r="D67" s="3">
+        <v>519295.076644897</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68">
+        <v>2010</v>
+      </c>
+      <c r="C68" s="3">
+        <v>64990.158908275</v>
+      </c>
+      <c r="D68" s="3">
+        <v>527850.69337192504</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69">
+        <v>2015</v>
+      </c>
+      <c r="C69" s="3">
+        <v>70173.092000000004</v>
+      </c>
+      <c r="D69" s="3">
+        <v>551180</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>25</v>
+      </c>
+      <c r="B70">
+        <v>2004</v>
+      </c>
+      <c r="C70" s="3">
+        <v>32950.982691076999</v>
+      </c>
+      <c r="D70" s="3">
+        <v>516471.68939628499</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>25</v>
+      </c>
+      <c r="B71">
+        <v>2007</v>
+      </c>
+      <c r="C71" s="3">
+        <v>42234.631679107799</v>
+      </c>
+      <c r="D71" s="3">
+        <v>517557.23491419997</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>25</v>
+      </c>
+      <c r="B72">
+        <v>2010</v>
+      </c>
+      <c r="C72" s="3">
+        <v>40484.483249093602</v>
+      </c>
+      <c r="D72" s="3">
+        <v>537067.41090004297</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>25</v>
+      </c>
+      <c r="B73">
+        <v>2015</v>
+      </c>
+      <c r="C73" s="3">
+        <v>45791.400999999998</v>
+      </c>
+      <c r="D73" s="3">
+        <v>547863</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74">
+        <v>2004</v>
+      </c>
+      <c r="C74" s="3">
+        <v>134314.195214323</v>
+      </c>
+      <c r="D74" s="3">
+        <v>785707.51922438899</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75">
+        <v>2007</v>
+      </c>
+      <c r="C75" s="3">
+        <v>142330.77649113</v>
+      </c>
+      <c r="D75" s="3">
+        <v>799411.46821294399</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>10</v>
+      </c>
+      <c r="B76">
+        <v>2010</v>
+      </c>
+      <c r="C76" s="3">
+        <v>135955.36908458799</v>
+      </c>
+      <c r="D76" s="3">
+        <v>817929.23565902002</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>10</v>
+      </c>
+      <c r="B77">
+        <v>2015</v>
+      </c>
+      <c r="C77" s="3">
+        <v>145254.44899999999</v>
+      </c>
+      <c r="D77" s="3">
+        <v>844505</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>22</v>
+      </c>
+      <c r="B78">
+        <v>2004</v>
+      </c>
+      <c r="C78" s="3">
+        <v>56138.8802292439</v>
+      </c>
+      <c r="D78" s="3">
+        <v>626104.54800358496</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>22</v>
+      </c>
+      <c r="B79">
+        <v>2007</v>
+      </c>
+      <c r="C79" s="3">
+        <v>66425.467834391806</v>
+      </c>
+      <c r="D79" s="3">
+        <v>639699.43673102895</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>22</v>
+      </c>
+      <c r="B80">
+        <v>2010</v>
+      </c>
+      <c r="C80" s="3">
+        <v>65807.901527814596</v>
+      </c>
+      <c r="D80" s="3">
+        <v>654957.10715914902</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>22</v>
+      </c>
+      <c r="B81">
+        <v>2015</v>
+      </c>
+      <c r="C81" s="3">
+        <v>68562.361999999994</v>
+      </c>
+      <c r="D81" s="3">
+        <v>676778</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>15</v>
+      </c>
+      <c r="B82">
+        <v>2004</v>
+      </c>
+      <c r="C82" s="3">
+        <v>70665.093726352396</v>
+      </c>
+      <c r="D82" s="3">
+        <v>541130</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>15</v>
+      </c>
+      <c r="B83">
+        <v>2007</v>
+      </c>
+      <c r="C83" s="3">
+        <v>79585</v>
+      </c>
+      <c r="D83" s="3">
+        <v>544548</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>15</v>
+      </c>
+      <c r="B84">
+        <v>2010</v>
+      </c>
+      <c r="C84" s="3">
+        <v>78770</v>
+      </c>
+      <c r="D84" s="3">
+        <v>557204</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>15</v>
+      </c>
+      <c r="B85">
+        <v>2015</v>
+      </c>
+      <c r="C85" s="3">
+        <v>84582.941999999995</v>
+      </c>
+      <c r="D85" s="3">
+        <v>572325</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>11</v>
+      </c>
+      <c r="B86">
+        <v>2004</v>
+      </c>
+      <c r="C86" s="3">
+        <v>118850.73036061</v>
+      </c>
+      <c r="D86" s="3">
+        <v>767289.17341040506</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>11</v>
+      </c>
+      <c r="B87">
+        <v>2007</v>
+      </c>
+      <c r="C87" s="3">
+        <v>123610.19942196499</v>
+      </c>
+      <c r="D87" s="3">
+        <v>773954.79364161799</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>11</v>
+      </c>
+      <c r="B88">
+        <v>2010</v>
+      </c>
+      <c r="C88" s="3">
+        <v>122591.50867051999</v>
+      </c>
+      <c r="D88" s="3">
+        <v>776396.04797687905</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>11</v>
+      </c>
+      <c r="B89">
+        <v>2015</v>
+      </c>
+      <c r="C89" s="3">
+        <v>130838.175</v>
+      </c>
+      <c r="D89" s="3">
+        <v>802126</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>9</v>
+      </c>
+      <c r="B90">
+        <v>2004</v>
+      </c>
+      <c r="C90" s="3">
+        <v>123348.33659626399</v>
+      </c>
+      <c r="D90" s="3">
+        <v>711582.43685238704</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>9</v>
+      </c>
+      <c r="B91">
+        <v>2007</v>
+      </c>
+      <c r="C91" s="3">
+        <v>141922.32577792901</v>
+      </c>
+      <c r="D91" s="3">
+        <v>714778.67854553601</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>9</v>
+      </c>
+      <c r="B92">
+        <v>2010</v>
+      </c>
+      <c r="C92" s="3">
+        <v>138426.974473501</v>
+      </c>
+      <c r="D92" s="3">
+        <v>718096.16867472604</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>9</v>
+      </c>
+      <c r="B93">
+        <v>2015</v>
+      </c>
+      <c r="C93" s="3">
+        <v>147433.94099999999</v>
+      </c>
+      <c r="D93" s="3">
+        <v>753762</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>17</v>
+      </c>
+      <c r="B94">
+        <v>2004</v>
+      </c>
+      <c r="C94" s="3">
+        <v>80183.096025661594</v>
+      </c>
+      <c r="D94" s="3">
+        <v>683912.57270956598</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>17</v>
+      </c>
+      <c r="B95">
+        <v>2006</v>
+      </c>
+      <c r="C95" s="3">
+        <v>79233.992398794595</v>
+      </c>
+      <c r="D95" s="3">
+        <v>698262.93332065595</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>17</v>
+      </c>
+      <c r="B96">
+        <v>2009</v>
+      </c>
+      <c r="C96" s="3">
+        <v>88180.489318030202</v>
+      </c>
+      <c r="D96" s="3">
+        <v>731125.76725603896</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>17</v>
+      </c>
+      <c r="B97">
+        <v>2012</v>
+      </c>
+      <c r="C97" s="3">
+        <v>83140.706832804703</v>
+      </c>
+      <c r="D97" s="3">
+        <v>775604.01349693502</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>17</v>
+      </c>
+      <c r="B98">
+        <v>2016</v>
+      </c>
+      <c r="C98" s="3">
+        <v>65930</v>
+      </c>
+      <c r="D98" s="3">
+        <v>685057</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>4</v>
+      </c>
+      <c r="B99">
+        <v>2004</v>
+      </c>
+      <c r="C99" s="3">
+        <v>261927.10589909201</v>
+      </c>
+      <c r="D99" s="3">
+        <v>1318540.6240067401</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>4</v>
+      </c>
+      <c r="B100">
+        <v>2006</v>
+      </c>
+      <c r="C100" s="3">
+        <v>240784.241460149</v>
+      </c>
+      <c r="D100" s="3">
+        <v>1333034.31383608</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>4</v>
+      </c>
+      <c r="B101">
+        <v>2009</v>
+      </c>
+      <c r="C101" s="3">
+        <v>259415.54067630999</v>
+      </c>
+      <c r="D101" s="3">
+        <v>1357880.7550813099</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102">
+        <v>2012</v>
+      </c>
+      <c r="C102" s="3">
+        <v>229694.10567757301</v>
+      </c>
+      <c r="D102" s="3">
+        <v>1393940.46503809</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>4</v>
+      </c>
+      <c r="B103">
+        <v>2016</v>
+      </c>
+      <c r="C103" s="3">
+        <v>197030</v>
+      </c>
+      <c r="D103" s="3">
+        <v>1256435</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I103"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1">
+        <v>2004</v>
+      </c>
+      <c r="C1">
+        <v>2006</v>
+      </c>
+      <c r="D1">
+        <v>2007</v>
+      </c>
+      <c r="E1">
+        <v>2009</v>
+      </c>
+      <c r="F1">
+        <v>2010</v>
+      </c>
+      <c r="G1">
+        <v>2012</v>
+      </c>
+      <c r="H1">
+        <v>2015</v>
+      </c>
+      <c r="I1">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.85956381861419295</v>
+      </c>
+      <c r="D2">
+        <v>0.81976102373728799</v>
+      </c>
+      <c r="F2">
+        <v>0.77127455464826999</v>
+      </c>
+      <c r="H2">
+        <v>0.81456721863769999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.804204508750331</v>
+      </c>
+      <c r="D3">
+        <v>0.87840758180770295</v>
+      </c>
+      <c r="F3">
+        <v>0.85921572605279894</v>
+      </c>
+      <c r="H3">
+        <v>0.82290159990689005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.90769965258462704</v>
+      </c>
+      <c r="D4">
+        <v>0.88977914300851302</v>
+      </c>
+      <c r="F4">
+        <v>0.92722660684454605</v>
+      </c>
+      <c r="H4">
+        <v>0.94432666514647001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.898712009493569</v>
+      </c>
+      <c r="C5">
+        <v>0.876658972484743</v>
+      </c>
+      <c r="E5">
+        <v>0.84516590421847204</v>
+      </c>
+      <c r="G5">
+        <v>0.88158182286264697</v>
+      </c>
+      <c r="I5">
+        <v>0.91068021040724201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.70285182046584105</v>
+      </c>
+      <c r="D6">
+        <v>0.70232751916931002</v>
+      </c>
+      <c r="F6">
+        <v>0.68918263531791402</v>
+      </c>
+      <c r="H6">
+        <v>0.80003768283063403</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.90877217030556001</v>
+      </c>
+      <c r="D7">
+        <v>0.88144664496451097</v>
+      </c>
+      <c r="F7">
+        <v>0.80785482801335695</v>
+      </c>
+      <c r="H7">
+        <v>0.87904579589960796</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.89775617306438504</v>
+      </c>
+      <c r="D8">
+        <v>0.92479478327134301</v>
+      </c>
+      <c r="F8">
+        <v>0.91629164545733599</v>
+      </c>
+      <c r="H8">
+        <v>0.88557810020803995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.51488638123234098</v>
+      </c>
+      <c r="D9">
+        <v>0.56382658847654799</v>
+      </c>
+      <c r="F9">
+        <v>0.70058371051898305</v>
+      </c>
+      <c r="H9">
+        <v>0.64422476627277603</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.88847462510944897</v>
+      </c>
+      <c r="D10">
+        <v>0.94097844050623602</v>
+      </c>
+      <c r="F10">
+        <v>0.90361589558001199</v>
+      </c>
+      <c r="H10">
+        <v>0.89963849895838399</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.85798752658034305</v>
+      </c>
+      <c r="D11">
+        <v>0.83097277891537402</v>
+      </c>
+      <c r="F11">
+        <v>0.78475536253974398</v>
+      </c>
+      <c r="H11">
+        <v>0.73778025841898298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.80174912882360505</v>
+      </c>
+      <c r="D12">
+        <v>0.85050558029580903</v>
+      </c>
+      <c r="F12">
+        <v>0.83198510734073905</v>
+      </c>
+      <c r="H12">
+        <v>0.77965636637288005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>-8.8310201893040299E-2</v>
+      </c>
+      <c r="D13">
+        <v>-0.112349329545777</v>
+      </c>
+      <c r="F13">
+        <v>-1.02390636226307E-2</v>
+      </c>
+      <c r="H13">
+        <v>0.12752090459762599</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.22032950241867599</v>
+      </c>
+      <c r="C14">
+        <v>0.134606089411234</v>
+      </c>
+      <c r="E14">
+        <v>4.2101605952084203E-2</v>
+      </c>
+      <c r="G14">
+        <v>8.7655740599478695E-3</v>
+      </c>
+      <c r="I14">
+        <v>0.18450216595100499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.89992872162297799</v>
+      </c>
+      <c r="D15">
+        <v>0.85491426195562703</v>
+      </c>
+      <c r="F15">
+        <v>0.86857608041445</v>
+      </c>
+      <c r="H15">
+        <v>0.83323660809254196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.83456736933714404</v>
+      </c>
+      <c r="D16">
+        <v>0.90024313369558095</v>
+      </c>
+      <c r="F16">
+        <v>0.88252201688075704</v>
+      </c>
+      <c r="H16">
+        <v>0.82726701225518295</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1">
+        <v>-6.5303563227485997E-2</v>
+      </c>
+      <c r="D17">
+        <v>1.7439499734143101E-2</v>
+      </c>
+      <c r="F17">
+        <v>-0.14152010519799799</v>
+      </c>
+      <c r="H17">
+        <v>-0.218924136269699</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.806803192098974</v>
+      </c>
+      <c r="D18">
+        <v>0.78924369510141701</v>
+      </c>
+      <c r="F18">
+        <v>0.77001683697149903</v>
+      </c>
+      <c r="H18">
+        <v>0.86099215142192298</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.46023355986638398</v>
+      </c>
+      <c r="D19">
+        <v>0.25097597260267501</v>
+      </c>
+      <c r="F19">
+        <v>0.30305998553529501</v>
+      </c>
+      <c r="H19">
+        <v>0.20526151845736801</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.72095251072293198</v>
+      </c>
+      <c r="D20">
+        <v>0.72556788910463099</v>
+      </c>
+      <c r="F20">
+        <v>0.76879542101365905</v>
+      </c>
+      <c r="H20">
+        <v>0.87990620909033701</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.59339829747544404</v>
+      </c>
+      <c r="D21">
+        <v>0.52881329466673799</v>
+      </c>
+      <c r="F21">
+        <v>0.447275964415347</v>
+      </c>
+      <c r="H21">
+        <v>0.45193787202075902</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.77020361078490196</v>
+      </c>
+      <c r="D22">
+        <v>0.71615320789820303</v>
+      </c>
+      <c r="F22">
+        <v>0.55735097598276395</v>
+      </c>
+      <c r="H22">
+        <v>0.628046641084266</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.26145939841565602</v>
+      </c>
+      <c r="D23">
+        <v>0.22407082210952001</v>
+      </c>
+      <c r="F23">
+        <v>0.30556951677037703</v>
+      </c>
+      <c r="H23">
+        <v>0.33888198813666598</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.79184544137449697</v>
+      </c>
+      <c r="D24">
+        <v>0.71048085738923195</v>
+      </c>
+      <c r="F24">
+        <v>0.74987385390219197</v>
+      </c>
+      <c r="H24">
+        <v>0.79887159571381705</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.57953084822227496</v>
+      </c>
+      <c r="D25">
+        <v>0.69823218964594103</v>
+      </c>
+      <c r="F25">
+        <v>0.70791092498831398</v>
+      </c>
+      <c r="H25">
+        <v>0.62301725590586998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.50830572335217905</v>
+      </c>
+      <c r="D26">
+        <v>0.38859454840096602</v>
+      </c>
+      <c r="F26">
+        <v>0.58316473315367101</v>
+      </c>
+      <c r="H26">
+        <v>0.38356320654202503</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="1"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B101" s="1"/>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B102" s="1"/>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B103" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add cor between deciles in 2004 to tables .xlsx
</commit_message>
<xml_diff>
--- a/tables/tables.xlsx
+++ b/tables/tables.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="prop_id_by_ttwa" sheetId="1" r:id="rId1"/>
     <sheet name="rci_by_year_place" sheetId="2" r:id="rId2"/>
     <sheet name="ttwa_pop_sizes" sheetId="4" r:id="rId3"/>
-    <sheet name="cor_between_rci_rdi" sheetId="3" r:id="rId4"/>
+    <sheet name="cor_between_deciles_2004" sheetId="5" r:id="rId4"/>
+    <sheet name="cor_between_rci_rdi" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="38">
   <si>
     <t>2006-2007</t>
   </si>
@@ -129,6 +130,9 @@
   <si>
     <t>pop_total</t>
   </si>
+  <si>
+    <t>correlation</t>
+  </si>
 </sst>
 </file>
 
@@ -138,9 +142,9 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +153,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -177,11 +189,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3030,7 +3043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -4487,6 +4500,234 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G11:G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>0.64626776241383899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>0.51940165757024404</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0.327954545454545</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>0.57357744372737296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>0.495441913022233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.40728729552620102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.31425921596898798</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>0.32004240407192502</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>0.39199445343193901</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>0.57507866789038897</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0.44166413867822302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>0.57847595300687304</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>0.30441036457015502</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>0.45021868502186801</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>0.52141613730759795</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>0.49430876799916001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>0.26728511912612402</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>0.40050160126557899</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>0.227585132302113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>0.29120674555308002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22">
+        <v>8.3262500461953506E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23">
+        <v>0.16108247706968501</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>0.36855944827945902</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <v>0.36576192782945</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>-4.4026463032691698E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I103"/>
   <sheetViews>

</xml_diff>